<commit_message>
Manually Comparing LLMs for final result
</commit_message>
<xml_diff>
--- a/analysis_results/o4_mini_Test00_20250526_160239/analysis_o4_mini_Test00_20250526_160239.xlsx
+++ b/analysis_results/o4_mini_Test00_20250526_160239/analysis_o4_mini_Test00_20250526_160239.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samso\Documents\Programming\AI_flaky_test\AI_flaky_test_detection\analysis_results\o4_mini_Test00_20250526_160239\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5431AEAF-0199-49F2-850D-46F1DA4231F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AB0566-2DB8-4C99-B085-4E4AE80B5365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5790" yWindow="-21720" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-1240" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
   <si>
     <t>Test Case</t>
   </si>
@@ -130,13 +130,7 @@
     <t>The LLM's fix replaces the existing sleep loops with a more robust waiting mechanism including a timeout. The developer's solution, however, adds assertions to check the buffer's internal counters (successful and dropped events) after waiting, which is a completely different approach and addresses the expected outcome of the backpressure strategy rather than just the waiting mechanism itself. The LLM's fix does not include these crucial assertions added by the developer.</t>
   </si>
   <si>
-    <t>tests_test_api.py_TestFootprint_test_flight_two_way</t>
-  </si>
-  <si>
     <t>OD-Brit</t>
-  </si>
-  <si>
-    <t>The original test code is empty, and the developer's fix adds the complete test file content. The LLM's proposed fix is an empty diff, indicating no changes were made or proposed. It completely misses the developer's solution of adding the missing test code.</t>
   </si>
   <si>
     <t>tests_test_hosts.py_TestHost_test_host_enable</t>
@@ -182,7 +176,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +188,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -231,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -240,6 +241,10 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -257,6 +262,204 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>468069</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>165274</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>477789</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>174634</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Encre 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{586E5ACF-55F2-222C-4EA0-C587A786CFE7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="3820680" y="2834160"/>
+            <a:ext cx="9720" cy="9360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Encre 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{586E5ACF-55F2-222C-4EA0-C587A786CFE7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3812040" y="2825520"/>
+              <a:ext cx="27360" cy="27000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2991960</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>256011</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3618182</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>381291</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="3" name="Encre 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81215275-8F78-104E-64FB-3D04B47798F2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="2991960" y="3306840"/>
+            <a:ext cx="624960" cy="125280"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="3" name="Encre 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81215275-8F78-104E-64FB-3D04B47798F2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2985840" y="3300720"/>
+              <a:ext cx="637200" cy="137520"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-05-27T15:32:09.932"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">27 26 17207 0 0,'0'0'0'0'0,"-3"-8"-1903"0"0,-7 3-409 0 0,5-4-352 0 0,-3 6-3128 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-05-27T15:32:14.951"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 348 5664 0 0,'34'-5'274'0'0,"241"-41"128"0"0,-195 30-342 0 0,-37 7-65 0 0,19-2-21 0 0,80-27-1 0 0,-92 24 11 0 0,97-16-1 0 0,-12 5-4 0 0,-95 16-7 0 0,50-2-1 0 0,-61 8 38 0 0,1-1-1 0 0,-1-1 1 0 0,52-16-1 0 0,-57 14-1 0 0,-1 1 0 0 0,1 1 0 0 0,0 1-1 0 0,0 1 1 0 0,0 2 0 0 0,27 0 0 0 0,28-2 26 0 0,-68 0-21 0 0,0 0-1 0 0,0 0 0 0 0,0-1 0 0 0,0-1 1 0 0,-1 0-1 0 0,11-6 0 0 0,-2 0-15 0 0,-12 7-101 0 0,1 1-1 0 0,-1-1 0 0 0,1 1 1 0 0,0 1-1 0 0,-1-1 1 0 0,2 1-1 0 0,-1 1 0 0 0,0 0 1 0 0,10-1-1 0 0,-16 2-2827 0 0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -546,13 +749,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="87" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.28515625" customWidth="1"/>
+    <col min="1" max="1" width="75.42578125" customWidth="1"/>
     <col min="2" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="208.5703125" style="3" customWidth="1"/>
@@ -711,20 +914,20 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="5" t="s">
         <v>28</v>
       </c>
     </row>
@@ -779,29 +982,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -810,32 +996,29 @@
         <v>8</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
       <c r="E16" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -844,32 +1027,32 @@
         <v>8</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -878,15 +1061,15 @@
         <v>8</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -895,10 +1078,11 @@
         <v>8</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>